<commit_message>
Chapter 1 math done. Speed triangles might be adjusted
Chapter 1 math done. Speed triangles might be adjusted
</commit_message>
<xml_diff>
--- a/docs/Hours.xlsx
+++ b/docs/Hours.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF10896-2D62-4726-9A33-4D16341FDE94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406D9374-0478-4C0C-9D6D-9F40006CCC44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>2019.02.19</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Chapter one math</t>
+  </si>
+  <si>
+    <t>2019.03.09</t>
+  </si>
+  <si>
+    <t>Speed triangles</t>
   </si>
 </sst>
 </file>
@@ -439,11 +445,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,6 +691,57 @@
         <v>31</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Chapter 1 finished. Chapter 2 started.
Chapter 1 finished. Chapter 2 started.
</commit_message>
<xml_diff>
--- a/docs/Hours.xlsx
+++ b/docs/Hours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406D9374-0478-4C0C-9D6D-9F40006CCC44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036197FF-36AA-433A-8D61-DE6793BB22BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>2019.02.19</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Speed triangles</t>
+  </si>
+  <si>
+    <t>2019.03.17</t>
+  </si>
+  <si>
+    <t>Hub calculations</t>
   </si>
 </sst>
 </file>
@@ -162,9 +168,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,11 +450,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +542,7 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
@@ -554,7 +559,7 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
@@ -571,7 +576,7 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
@@ -588,7 +593,7 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>0.5</v>
       </c>
     </row>
@@ -602,7 +607,7 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>1</v>
       </c>
     </row>
@@ -616,7 +621,7 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
@@ -633,7 +638,7 @@
       <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
@@ -650,7 +655,7 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
@@ -667,7 +672,7 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
@@ -684,7 +689,7 @@
       <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
@@ -701,7 +706,7 @@
       <c r="C15" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
@@ -718,7 +723,7 @@
       <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
@@ -727,7 +732,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>32</v>
@@ -735,11 +740,28 @@
       <c r="C17" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update variables replaced by values.
Update variables replaced by values.
</commit_message>
<xml_diff>
--- a/docs/Hours.xlsx
+++ b/docs/Hours.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F80F45D-F055-464F-9688-76E3E7F30630}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26589186-3545-451E-8842-7B2FACB36B95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>2019.02.19</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>Import points and prepare simulation</t>
+  </si>
+  <si>
+    <t>2019.04.09</t>
+  </si>
+  <si>
+    <t>Ansys Fluent simulation</t>
+  </si>
+  <si>
+    <t>2019.04.14</t>
+  </si>
+  <si>
+    <t>Added numerics to equation for better following</t>
   </si>
 </sst>
 </file>
@@ -489,18 +501,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -941,7 +953,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>45</v>
@@ -958,7 +970,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>45</v>
@@ -971,6 +983,45 @@
       </c>
       <c r="E28" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>2.5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>